<commit_message>
RHI plots with the position of the sphere added
</commit_message>
<xml_diff>
--- a/Post_processing/Tables_after_wr_wb/Table_exp1.xlsx
+++ b/Post_processing/Tables_after_wr_wb/Table_exp1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Datetime</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Wb y</t>
+  </si>
+  <si>
+    <t>Exp Constant</t>
+  </si>
+  <si>
+    <t>Exp Constant [dB]</t>
   </si>
   <si>
     <t>2022-05-07  17:51:13</t>
@@ -458,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,16 +546,22 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>27.1</v>
@@ -620,16 +632,22 @@
       <c r="Z2">
         <v>0.2429725417096719</v>
       </c>
+      <c r="AA2">
+        <v>385250961.9682089</v>
+      </c>
+      <c r="AB2">
+        <v>85.85743731821252</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>216.8</v>
@@ -700,16 +718,22 @@
       <c r="Z3">
         <v>0.4500004706293059</v>
       </c>
+      <c r="AA3">
+        <v>385250961.9682089</v>
+      </c>
+      <c r="AB3">
+        <v>85.85743731821252</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>12.36</v>
@@ -779,6 +803,12 @@
       </c>
       <c r="Z4">
         <v>0.1332608696881664</v>
+      </c>
+      <c r="AA4">
+        <v>385250961.9682089</v>
+      </c>
+      <c r="AB4">
+        <v>85.85743731821252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>